<commit_message>
updated leaflet to most current rx_west.shp
</commit_message>
<xml_diff>
--- a/Database Structure.xlsx
+++ b/Database Structure.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\WesternDryForestsAndFireInititative\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PRJ\StateRx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B7AF26-63D8-412E-B0C7-752AE7FFC5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9B7E8D-F544-4489-B76D-F2143E17420B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{0044F328-7436-4CA7-892D-6488E67CD075}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{0044F328-7436-4CA7-892D-6488E67CD075}"/>
   </bookViews>
   <sheets>
-    <sheet name="structure (2)" sheetId="3" r:id="rId1"/>
-    <sheet name="structure" sheetId="1" r:id="rId2"/>
-    <sheet name="state attributes" sheetId="2" r:id="rId3"/>
+    <sheet name="simple" sheetId="4" r:id="rId1"/>
+    <sheet name="structure (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="structure" sheetId="1" r:id="rId3"/>
+    <sheet name="state attributes" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="143">
   <si>
     <t>IN_NFPORS</t>
   </si>
@@ -548,12 +549,39 @@
   <si>
     <t>Total tons. Calculated as tons * completed acres if reported as tons/acres.</t>
   </si>
+  <si>
+    <t>Acres permitted</t>
+  </si>
+  <si>
+    <t>Acres completed</t>
+  </si>
+  <si>
+    <t>Pile volume</t>
+  </si>
+  <si>
+    <t>Burn name</t>
+  </si>
+  <si>
+    <t>Burn type</t>
+  </si>
+  <si>
+    <t>Entity reqeusting</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>DATABASE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -588,6 +616,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -615,7 +658,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -623,11 +666,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -640,6 +698,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -975,10 +1035,95 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EEBADD0-DCCE-4367-8842-9C39E9DC6A72}">
+  <dimension ref="B2:C34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="26.77734375" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" style="7" customWidth="1"/>
+    <col min="4" max="5" width="26.77734375" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="B3" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="B4" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="B5" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="B6" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="B7" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="B8" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="B9" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="B10" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="B11" s="10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="B12" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+      <c r="C18" s="8"/>
+    </row>
+    <row r="32" spans="2:3" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="33" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="34" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB0E950-1393-4D0F-BFD2-F3EC61E3DCB6}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -1415,7 +1560,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB16F03E-2F40-4FCE-8F95-8D8B443534AA}">
   <dimension ref="A1:D36"/>
   <sheetViews>
@@ -1848,7 +1993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86214E37-BAFD-4345-86D6-07B1D896F87F}">
   <dimension ref="A1:F14"/>
   <sheetViews>

</xml_diff>

<commit_message>
intersected tnc points with state permits
</commit_message>
<xml_diff>
--- a/Database Structure.xlsx
+++ b/Database Structure.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PRJ\StateRx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9B7E8D-F544-4489-B76D-F2143E17420B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB868D6-D291-4A27-9E30-71A4CD92F788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{0044F328-7436-4CA7-892D-6488E67CD075}"/>
   </bookViews>
   <sheets>
-    <sheet name="simple" sheetId="4" r:id="rId1"/>
-    <sheet name="structure (2)" sheetId="3" r:id="rId2"/>
-    <sheet name="structure" sheetId="1" r:id="rId3"/>
-    <sheet name="state attributes" sheetId="2" r:id="rId4"/>
+    <sheet name="structure (2)" sheetId="3" r:id="rId1"/>
+    <sheet name="structure" sheetId="1" r:id="rId2"/>
+    <sheet name="state attributes" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -75,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="134">
   <si>
     <t>IN_NFPORS</t>
   </si>
@@ -549,39 +548,12 @@
   <si>
     <t>Total tons. Calculated as tons * completed acres if reported as tons/acres.</t>
   </si>
-  <si>
-    <t>Acres permitted</t>
-  </si>
-  <si>
-    <t>Acres completed</t>
-  </si>
-  <si>
-    <t>Pile volume</t>
-  </si>
-  <si>
-    <t>Burn name</t>
-  </si>
-  <si>
-    <t>Burn type</t>
-  </si>
-  <si>
-    <t>Entity reqeusting</t>
-  </si>
-  <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>DATABASE</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -616,21 +588,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -658,7 +615,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -666,26 +623,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -698,8 +640,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1035,95 +975,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EEBADD0-DCCE-4367-8842-9C39E9DC6A72}">
-  <dimension ref="B2:C34"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="26.77734375" customWidth="1"/>
-    <col min="3" max="3" width="26.77734375" style="7" customWidth="1"/>
-    <col min="4" max="5" width="26.77734375" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C2" s="8"/>
-    </row>
-    <row r="3" spans="2:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="B3" s="11" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="B4" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="B5" s="10" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="B6" s="10" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="B7" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="B8" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="2:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="B9" s="10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="B10" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="B11" s="10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="B12" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="2"/>
-      <c r="C18" s="8"/>
-    </row>
-    <row r="32" spans="2:3" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="33" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="34" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB0E950-1393-4D0F-BFD2-F3EC61E3DCB6}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -1560,12 +1415,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB16F03E-2F40-4FCE-8F95-8D8B443534AA}">
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1993,12 +1848,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86214E37-BAFD-4345-86D6-07B1D896F87F}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>